<commit_message>
Ver3 corrected some things in all 3 furniture files.
</commit_message>
<xml_diff>
--- a/Test_Specification_Exercise1_Furniture_Sale.xlsx
+++ b/Test_Specification_Exercise1_Furniture_Sale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X\Desktop\Testing_exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167646CA-20A4-47A1-B482-3C1DBB5276E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7826DF7B-8E16-4043-A0ED-1552CB7A846C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{834C1BAD-FEC9-46B1-8019-162670ECADF2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="91">
   <si>
     <t>total (Decimal - Precision 2):</t>
   </si>
@@ -43,9 +43,6 @@
     <t>day</t>
   </si>
   <si>
-    <t>result</t>
-  </si>
-  <si>
     <t>vEP1(1):</t>
   </si>
   <si>
@@ -88,12 +85,6 @@
     <t>Bonus +10%</t>
   </si>
   <si>
-    <t>[27.12.2022,..,MAX_DATE]</t>
-  </si>
-  <si>
-    <t>[26.11.2022, 28.11.2022,.., 03.12.2022, 05.12.2022,.., 07.12.2022, 09.12.2022, 10.12.2022, 12.12.2022,.., 17.12.2022, 19.12.2022,.., 24.12.2022]</t>
-  </si>
-  <si>
     <t>[28.11.2022,.., 02.12.2022, 05.12.2022,.., 07.12.2022, 09.12.2022, 12.12.2022,.., 16.12.2022, 19.12.2022,.., 23.12.2022]</t>
   </si>
   <si>
@@ -259,9 +250,6 @@
     <t>Decimal("-1000.00")</t>
   </si>
   <si>
-    <t>side notes (ignore)</t>
-  </si>
-  <si>
     <t>Kleinster realistischer Betrag</t>
   </si>
   <si>
@@ -271,9 +259,6 @@
     <t>Mittig</t>
   </si>
   <si>
-    <t>Einfacher String</t>
-  </si>
-  <si>
     <t>4 Ziffern negativ</t>
   </si>
   <si>
@@ -292,15 +277,6 @@
     <t>Decimal("0.2")</t>
   </si>
   <si>
-    <t>Decimal("0.2")+Decimal("0.1")-(Decimal("0.2")*Decimal("0.1"))</t>
-  </si>
-  <si>
-    <t>Decimal("0.1")+Decimal("0.1")-(Decimal("0.1")*Decimal("0.1"))</t>
-  </si>
-  <si>
-    <t>Decimal("0.05")+Decimal("0.1")-(Decimal("0.05")*Decimal("0.1"))</t>
-  </si>
-  <si>
     <t>[100.00,..,"500.00"[</t>
   </si>
   <si>
@@ -311,6 +287,24 @@
   </si>
   <si>
     <t>10*8+3+3=86(+1 extra = 87)</t>
+  </si>
+  <si>
+    <t>Einfacher String für total</t>
+  </si>
+  <si>
+    <t>Einfacher String für day</t>
+  </si>
+  <si>
+    <t>Decimal("0.05")+Decimal("0.1")-(Decimal("0.05")*Decimal("0.1"))=0.15</t>
+  </si>
+  <si>
+    <t>result (Decimal - precision 2 - Round_Half_Up)</t>
+  </si>
+  <si>
+    <t>Decimal("0.1")+Decimal("0.1")-(Decimal("0.1")*Decimal("0.1"))=0.19</t>
+  </si>
+  <si>
+    <t>Decimal("0.2")+Decimal("0.1")-(Decimal("0.2")*Decimal("0.1"))=0.28</t>
   </si>
 </sst>
 </file>
@@ -760,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52D8ACF-31DD-45C4-876D-5883C18EED61}">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,13 +775,13 @@
       </c>
       <c r="B1" s="16"/>
       <c r="H1" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -799,10 +793,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -813,19 +807,19 @@
         <v>0.05</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -836,19 +830,19 @@
         <v>0.1</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -859,10 +853,10 @@
         <v>0.2</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K5" s="3"/>
     </row>
@@ -872,10 +866,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -883,22 +877,22 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -906,13 +900,13 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -922,7 +916,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -934,10 +928,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -948,10 +942,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -959,10 +953,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -970,13 +964,13 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -984,10 +978,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -995,13 +989,13 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1013,10 +1007,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1024,22 +1018,22 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1047,36 +1041,36 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K17" s="6"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19" s="18"/>
       <c r="I19" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C20" s="17"/>
       <c r="I20" s="13"/>
@@ -1085,16 +1079,16 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I21" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K21" s="13"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1103,16 +1097,16 @@
       <c r="F22" s="3"/>
       <c r="H22" s="1"/>
       <c r="I22" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K22" s="13"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>1</v>
@@ -1121,15 +1115,15 @@
         <v>2</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="I23" s="14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K23" s="13"/>
     </row>
@@ -1138,21 +1132,21 @@
         <v>1</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="I24" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="K24" s="13"/>
     </row>
@@ -1161,21 +1155,21 @@
         <v>2</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="I25" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="K25" s="13"/>
     </row>
@@ -1184,21 +1178,21 @@
         <v>3</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="I26" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K26" s="13"/>
     </row>
@@ -1207,21 +1201,21 @@
         <v>4</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="I27" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K27" s="13"/>
     </row>
@@ -1230,21 +1224,21 @@
         <v>5</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="I28" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K28" s="13"/>
     </row>
@@ -1253,21 +1247,21 @@
         <v>6</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="I29" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="K29" s="13"/>
     </row>
@@ -1276,21 +1270,21 @@
         <v>7</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="I30" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K30" s="13"/>
     </row>
@@ -1299,13 +1293,13 @@
         <v>8</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1315,278 +1309,269 @@
         <v>9</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>10</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>11</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>12</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>13</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>14</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>15</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>16</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>17</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>18</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>19</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>20</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>21</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>22</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="I45" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>23</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="I46" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>24</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="I47" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>25</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -1596,13 +1581,13 @@
         <v>26</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -1612,13 +1597,13 @@
         <v>27</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -1628,13 +1613,13 @@
         <v>28</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -1644,13 +1629,13 @@
         <v>29</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -1660,13 +1645,13 @@
         <v>30</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -1676,13 +1661,13 @@
         <v>31</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -1692,13 +1677,13 @@
         <v>32</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -1708,13 +1693,13 @@
         <v>33</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -1724,13 +1709,13 @@
         <v>34</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -1740,13 +1725,13 @@
         <v>35</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -1756,13 +1741,13 @@
         <v>36</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -1772,13 +1757,13 @@
         <v>37</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -1788,13 +1773,13 @@
         <v>38</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -1804,13 +1789,13 @@
         <v>39</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -1820,13 +1805,13 @@
         <v>40</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -1836,13 +1821,13 @@
         <v>41</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -1852,13 +1837,13 @@
         <v>42</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -1868,13 +1853,13 @@
         <v>43</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -1884,13 +1869,13 @@
         <v>44</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -1900,13 +1885,13 @@
         <v>45</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
@@ -1916,13 +1901,13 @@
         <v>46</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
@@ -1932,13 +1917,13 @@
         <v>47</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -1948,13 +1933,13 @@
         <v>48</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
@@ -1964,13 +1949,13 @@
         <v>49</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -1980,13 +1965,13 @@
         <v>50</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -1996,13 +1981,13 @@
         <v>51</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -2012,13 +1997,13 @@
         <v>52</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
@@ -2028,13 +2013,13 @@
         <v>53</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
@@ -2044,13 +2029,13 @@
         <v>54</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
@@ -2060,13 +2045,13 @@
         <v>55</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
@@ -2076,13 +2061,13 @@
         <v>56</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
@@ -2092,13 +2077,13 @@
         <v>57</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
@@ -2108,13 +2093,13 @@
         <v>58</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
@@ -2124,13 +2109,13 @@
         <v>59</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
@@ -2140,13 +2125,13 @@
         <v>60</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
@@ -2156,13 +2141,13 @@
         <v>61</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
@@ -2172,13 +2157,13 @@
         <v>62</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
@@ -2188,13 +2173,13 @@
         <v>63</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
@@ -2204,13 +2189,13 @@
         <v>64</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
@@ -2220,13 +2205,13 @@
         <v>65</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
@@ -2236,13 +2221,13 @@
         <v>66</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
@@ -2252,13 +2237,13 @@
         <v>67</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
@@ -2268,13 +2253,13 @@
         <v>68</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
@@ -2284,13 +2269,13 @@
         <v>69</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
@@ -2300,13 +2285,13 @@
         <v>70</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
@@ -2316,13 +2301,13 @@
         <v>71</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
@@ -2332,13 +2317,13 @@
         <v>72</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
@@ -2348,13 +2333,13 @@
         <v>73</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
@@ -2364,13 +2349,13 @@
         <v>74</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
@@ -2380,13 +2365,13 @@
         <v>75</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
@@ -2396,13 +2381,13 @@
         <v>76</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
@@ -2412,13 +2397,13 @@
         <v>77</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
@@ -2428,13 +2413,13 @@
         <v>78</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
@@ -2444,13 +2429,13 @@
         <v>79</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
@@ -2460,13 +2445,13 @@
         <v>80</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
@@ -2476,13 +2461,13 @@
         <v>81</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E104" s="6"/>
       <c r="F104" s="6"/>
@@ -2492,13 +2477,13 @@
         <v>82</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E105" s="6"/>
       <c r="F105" s="6"/>
@@ -2508,13 +2493,13 @@
         <v>83</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D106" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E106" s="6"/>
       <c r="F106" s="6"/>
@@ -2524,13 +2509,13 @@
         <v>84</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E107" s="6"/>
       <c r="F107" s="6"/>
@@ -2540,13 +2525,13 @@
         <v>85</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E108" s="6"/>
       <c r="F108" s="6"/>
@@ -2556,13 +2541,13 @@
         <v>86</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E109" s="6"/>
       <c r="F109" s="6"/>
@@ -2572,13 +2557,13 @@
         <v>87</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E110" s="6"/>
       <c r="F110" s="6"/>

</xml_diff>